<commit_message>
Se actualiza codigo para lectura y comparación de documentos en archivo DataTest.java
</commit_message>
<xml_diff>
--- a/documents/procesedDocuments/TestData.xlsx
+++ b/documents/procesedDocuments/TestData.xlsx
@@ -23,34 +23,34 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
+    </style:style>
+    <style:style style:name="co2" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.011cm"/>
     </style:style>
-    <style:style style:name="co2" style:family="table-column">
+    <style:style style:name="co3" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.778cm"/>
     </style:style>
-    <style:style style:name="co3" style:family="table-column">
+    <style:style style:name="co4" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.528cm"/>
     </style:style>
-    <style:style style:name="co4" style:family="table-column">
+    <style:style style:name="co5" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="3.166cm"/>
     </style:style>
-    <style:style style:name="co5" style:family="table-column">
+    <style:style style:name="co6" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="1.071cm"/>
     </style:style>
-    <style:style style:name="co6" style:family="table-column">
+    <style:style style:name="co7" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.202cm"/>
     </style:style>
-    <style:style style:name="co7" style:family="table-column">
+    <style:style style:name="co8" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="3.847cm"/>
     </style:style>
-    <style:style style:name="co8" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
-    </style:style>
     <style:style style:name="ro1" style:family="table-row">
+      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro2" style:family="table-row">
       <style:table-row-properties style:row-height="0.487cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro2" style:family="table-row">
-      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -67,15 +67,45 @@
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
+      <table:table table:name="Hoja6" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+        </table:table-row>
+      </table:table>
+      <table:table table:name="Hoja5" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+        </table:table-row>
+      </table:table>
+      <table:table table:name="Hoja4" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+        </table:table-row>
+      </table:table>
+      <table:table table:name="Hoja3" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+        </table:table-row>
+      </table:table>
+      <table:table table:name="Hoja2" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+        </table:table-row>
+      </table:table>
       <table:table table:name="CER150" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co5" table:default-cell-style-name="ce2"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co7" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
-        <table:table-row table:style-name="ro1">
+        <table:table-column table:style-name="co5" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce2"/>
+        <table:table-column table:style-name="co7" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co8" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro2">
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Ciudad</text:p>
           </table:table-cell>
@@ -101,7 +131,7 @@
             <text:p>31/12/2021</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>AMAGA</text:p>
           </table:table-cell>
@@ -122,7 +152,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>APARTADo</text:p>
           </table:table-cell>
@@ -148,7 +178,7 @@
             <text:p>0,0396409871549027</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ARAUCA</text:p>
           </table:table-cell>
@@ -174,7 +204,7 @@
             <text:p>0,206340046814361</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ARRIEROS MEDELLiN</text:p>
           </table:table-cell>
@@ -195,7 +225,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>BARRANCABERMEJA</text:p>
           </table:table-cell>
@@ -221,7 +251,7 @@
             <text:p>0,111898793398022</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>BARRANQUILLA</text:p>
           </table:table-cell>
@@ -247,7 +277,7 @@
             <text:p>0,160683957459081</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>BELLO</text:p>
           </table:table-cell>
@@ -273,7 +303,7 @@
             <text:p>0,00816957081027624</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>BOGOTA</text:p>
           </table:table-cell>
@@ -299,7 +329,7 @@
             <text:p>0,020892495752522</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>BOGOTA</text:p>
           </table:table-cell>
@@ -335,11 +365,11 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.3">
   <office:meta>
-    <dc:date>2023-08-23T09:13:25.231000000</dc:date>
-    <meta:editing-duration>PT4M</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
+    <dc:date>2023-08-28T15:11:09.051000000</dc:date>
+    <meta:editing-duration>PT4M26S</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
     <meta:generator>LibreOffice/7.4.5.1$Windows_X86_64 LibreOffice_project/9c0871452b3918c1019dde9bfac75448afc4b57f</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="76" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="6" meta:cell-count="76" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -350,8 +380,8 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">26450</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">4551</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">2258</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">452</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -370,9 +400,79 @@
               <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
+            <config:config-item-map-entry config:name="Hoja2">
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
+            </config:config-item-map-entry>
+            <config:config-item-map-entry config:name="Hoja3">
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
+            </config:config-item-map-entry>
+            <config:config-item-map-entry config:name="Hoja4">
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
+            </config:config-item-map-entry>
+            <config:config-item-map-entry config:name="Hoja5">
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
+            </config:config-item-map-entry>
+            <config:config-item-map-entry config:name="Hoja6">
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">9</config:config-item>
+              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
+              <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
+              <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
+            </config:config-item-map-entry>
           </config:config-item-map-named>
-          <config:config-item config:name="ActiveTable" config:type="string">CER150</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1301</config:config-item>
+          <config:config-item config:name="ActiveTable" config:type="string">Hoja6</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1285</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -418,9 +518,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Snagit 12</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">1QT+/1NuYWdpdCAxMgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU25hZ2l0IDEyIFByaW50ZXIAAAAAAAAAAAAAAAAAAAAWAAEA8gMAAAAAAAAEAAhSAAAEdAAAM1ROVwAAAAAKAFMAbgBhAGcAaQB0ACAAMQAyAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAABBAMG3AAMA0PvgAUBAAkAmgs0CGQAAQAPAMgAAgABAMgAAgABAEEANAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAABAAAA/////wAAAAAAAAAAAAAAAAAAAABESU5VIgCwAAwDAADBlRz7AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAYAAAABAAAAAAAAAAIAAQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAsAAAAFNNVEoAAAAAEACgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAASAENPTVBBVF9EVVBMRVhfTU9ERRMARHVwbGV4TW9kZTo6VW5rbm93bg==</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -435,6 +535,21 @@
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
+        <config:config-item-map-entry config:name="Hoja6">
+          <config:config-item config:name="CodeName" config:type="string">Hoja6</config:config-item>
+        </config:config-item-map-entry>
+        <config:config-item-map-entry config:name="Hoja5">
+          <config:config-item config:name="CodeName" config:type="string">Hoja5</config:config-item>
+        </config:config-item-map-entry>
+        <config:config-item-map-entry config:name="Hoja4">
+          <config:config-item config:name="CodeName" config:type="string">Hoja4</config:config-item>
+        </config:config-item-map-entry>
+        <config:config-item-map-entry config:name="Hoja3">
+          <config:config-item config:name="CodeName" config:type="string">Hoja3</config:config-item>
+        </config:config-item-map-entry>
+        <config:config-item-map-entry config:name="Hoja2">
+          <config:config-item config:name="CodeName" config:type="string">Hoja2</config:config-item>
+        </config:config-item-map-entry>
         <config:config-item-map-entry config:name="CER150">
           <config:config-item config:name="CodeName" config:type="string">Hoja1</config:config-item>
         </config:config-item-map-entry>
@@ -460,20 +575,6 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:currency-style style:name="N107P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N107">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N107P0"/>
-    </number:currency-style>
     <number:currency-style style:name="N108P0" style:volatile="true">
       <number:currency-symbol/>
       <number:text> </number:text>
@@ -481,207 +582,215 @@
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N108">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N108P0"/>
+    </number:currency-style>
+    <number:number-style style:name="N117P0" style:volatile="true">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N117">
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N117P0"/>
+    </number:number-style>
+    <number:currency-style style:name="N109P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N109">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:text> </number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N108P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N109P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N109">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N109P0"/>
     </number:currency-style>
-    <number:currency-style style:name="N110P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N110">
+    <number:currency-style style:name="N111P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N111">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N111P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N112P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N112">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:text> </number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N110P0"/>
-    </number:currency-style>
-    <number:date-style style:name="N111">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N112P0"/>
+    </number:currency-style>
+    <number:date-style style:name="N113">
       <number:day number:style="long"/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N112">
+    <number:date-style style:name="N114">
       <number:day number:style="long"/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
     </number:date-style>
-    <number:date-style style:name="N113">
+    <number:date-style style:name="N115">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:number-style style:name="N114P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N114">
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N114P0"/>
-    </number:number-style>
-    <number:number-style style:name="N115P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N115">
+    <number:number-style style:name="N118P0" style:volatile="true">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N118">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N115P0"/>
-    </number:number-style>
-    <number:number-style style:name="N116P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N116">
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N116P0"/>
-    </number:number-style>
-    <number:number-style style:name="N117P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N117">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N118P0"/>
+    </number:number-style>
+    <number:number-style style:name="N120P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N120">
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N120P0"/>
+    </number:number-style>
+    <number:number-style style:name="N121P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N121">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N117P0"/>
-    </number:number-style>
-    <number:number-style style:name="N118P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N118P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N118P2" style:volatile="true">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
+    </number:number-style>
+    <number:number-style style:name="N125P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:number-style>
-    <number:text-style style:name="N118">
+    <number:text-style style:name="N125">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N118P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N118P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N118P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
     </number:text-style>
-    <number:currency-style style:name="N119P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N119P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N119P2" style:volatile="true">
-      <number:text> </number:text>
+    <number:currency-style style:name="N129P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N129P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N129P2" style:volatile="true">
       <number:currency-symbol/>
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>- </number:text>
     </number:currency-style>
-    <number:text-style style:name="N119">
+    <number:text-style style:name="N129">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N119P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N119P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N119P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N129P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N129P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N129P2"/>
     </number:text-style>
-    <number:number-style style:name="N120P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N120P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N120P2" style:volatile="true">
+    <number:number-style style:name="N133P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N133P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N133P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N120">
+    <number:text-style style:name="N133">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N120P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N120P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N120P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N133P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N133P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N133P2"/>
     </number:text-style>
-    <number:currency-style style:name="N121P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N121P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N121P2" style:volatile="true">
-      <number:text> </number:text>
+    <number:currency-style style:name="N137P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N137P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N137P2" style:volatile="true">
       <number:currency-symbol/>
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
@@ -689,32 +798,32 @@
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:currency-style>
-    <number:text-style style:name="N121">
+    <number:text-style style:name="N137">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N121P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N121P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N121P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N137P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N137P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N137P2"/>
     </number:text-style>
-    <number:time-style style:name="N122">
+    <number:time-style style:name="N138">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N123" number:truncate-on-overflow="false">
+    <number:time-style style:name="N139" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N124">
+    <number:time-style style:name="N140">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N125">
+    <number:number-style style:name="N141">
       <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell"/>

</xml_diff>